<commit_message>
All in One Test suite
</commit_message>
<xml_diff>
--- a/cypress/downloads/test.xlsx
+++ b/cypress/downloads/test.xlsx
@@ -15,63 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Reg</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Asset Group / Asset Type</t>
+    <t>Site Name</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Last Inspection Date</t>
-  </si>
-  <si>
-    <t>Next Inspection Date</t>
-  </si>
-  <si>
-    <t>Acquired Date</t>
-  </si>
-  <si>
-    <t>Date On Site</t>
-  </si>
-  <si>
-    <t>Date Off Hired</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Registration Status</t>
-  </si>
-  <si>
-    <t>Is Available For Datatouch</t>
+    <t>Is Available For All Sites</t>
   </si>
   <si>
     <t>Is Active</t>
   </si>
   <si>
-    <t>lok</t>
+    <t>Drive Meadow </t>
   </si>
   <si>
-    <t>Car Monday / Car Monday Type</t>
-  </si>
-  <si>
-    <t>Added Redesign QA Company </t>
-  </si>
-  <si>
-    <t>njjm</t>
-  </si>
-  <si>
-    <t>Pending</t>
+    <t>QA Site</t>
   </si>
   <si>
     <t>false</t>
@@ -84,9 +48,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-9]dd MMM yyyy"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -128,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" applyAlignment="1" fontId="1" applyNumberFormat="0" numFmtId="0">
       <alignment vertical="top" wrapText="1" horizontal="center"/>
     </xf>
@@ -142,9 +103,6 @@
       <alignment vertical="top" wrapText="1" horizontal="right"/>
     </xf>
     <xf xfId="0" applyAlignment="1" fontId="0" applyNumberFormat="0" numFmtId="0">
-      <alignment vertical="top" wrapText="1" horizontal="left"/>
-    </xf>
-    <xf xfId="0" applyAlignment="1" fontId="0" applyNumberFormat="1" numFmtId="165">
       <alignment vertical="top" wrapText="1" horizontal="left"/>
     </xf>
     <xf xfId="0" applyAlignment="1" fontId="0" applyNumberFormat="0" numFmtId="0">
@@ -172,22 +130,13 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col width="13.57" min="1" max="1" customWidth="1"/>
-    <col width="6.29" min="2" max="2" customWidth="1"/>
-    <col width="6.29" min="3" max="3" customWidth="1"/>
-    <col width="6.29" min="4" max="4" customWidth="1"/>
-    <col width="6.29" min="5" max="5" customWidth="1"/>
-    <col width="6.29" min="6" max="6" customWidth="1"/>
-    <col width="6.29" min="7" max="7" customWidth="1"/>
-    <col width="6.29" min="8" max="8" customWidth="1"/>
-    <col width="6.29" min="9" max="9" customWidth="1"/>
-    <col width="6.29" min="10" max="10" customWidth="1"/>
-    <col width="6.29" min="11" max="11" customWidth="1"/>
-    <col width="6.29" min="12" max="12" customWidth="1"/>
-    <col width="6.29" min="13" max="13" customWidth="1"/>
-    <col width="13.57" min="14" max="14" customWidth="1"/>
+    <col width="23.43" min="2" max="2" customWidth="1"/>
+    <col width="23.43" min="3" max="3" customWidth="1"/>
+    <col width="23.43" min="4" max="4" customWidth="1"/>
+    <col width="23.43" min="5" max="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -203,64 +152,22 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+    </row>
+    <row r="2" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="n">
+        <v>129709</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="n">
-        <v>133511</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="5" t="s"/>
-      <c r="F2" s="5" t="s"/>
-      <c r="G2" s="5" t="s"/>
-      <c r="H2" s="5" t="s"/>
-      <c r="I2" s="5" t="s"/>
-      <c r="J2" s="4" t="s"/>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>